<commit_message>
Add scripts and notebooks estimating covariant angular distributions
</commit_message>
<xml_diff>
--- a/Data/Data list.xlsx
+++ b/Data/Data list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daehyun/Dropbox/SACLA 2017B8065 Takanashi/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F62A3E0A-72B0-2E41-9B41-6CB38178380A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7877B3B9-C8D4-6548-9E1D-30753199145C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35620" yWindow="460" windowWidth="36380" windowHeight="16940" activeTab="1" xr2:uid="{8705D306-1A2C-FB42-8015-52B92150CBBB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{8705D306-1A2C-FB42-8015-52B92150CBBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="66">
   <si>
     <t>aq024</t>
   </si>
@@ -212,6 +212,24 @@
   </si>
   <si>
     <t>aq028, 029, 035, 036; Int-dependent cov KER; target={target} &amp; p={p} &amp; phi={h1phiy}.py</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>v20190511</t>
+  </si>
+  <si>
+    <t>v20190514</t>
+  </si>
+  <si>
+    <t>aq028, 029, 035, 036; Int-dependent cov ang dist and KER; target={target}.py</t>
+  </si>
+  <si>
+    <t>Cov ang dist and KER; target={target} &amp; gm2={fr:.3f}--{to:.3f}.pickle</t>
+  </si>
+  <si>
+    <t>v20190510</t>
   </si>
 </sst>
 </file>
@@ -260,7 +278,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="10">
     <dxf>
       <font>
         <b val="0"/>
@@ -277,7 +295,6 @@
         <name val="Menlo Regular"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -329,6 +346,24 @@
         <name val="Menlo Regular"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Menlo Regular"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <font>
@@ -440,13 +475,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C288E936-78ED-DC49-B351-61BAF435EDEE}" name="Table1" displayName="Table1" ref="A1:H17" totalsRowShown="0" headerRowDxfId="8">
-  <autoFilter ref="A1:H17" xr:uid="{B98D8822-403F-E442-BAE2-1B0B4CF679C4}"/>
-  <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{8CE13ACE-E9B8-3E47-8AF0-6D095CDC24CC}" name="target" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{51BF5B04-AEB1-434E-9660-5E7CFDD1FCEE}" name="flag" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{28841166-1611-7E4F-915D-75506BDADEB1}" name="p" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{19F13757-8028-F143-A57B-600899444B8A}" name="h0pz" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C288E936-78ED-DC49-B351-61BAF435EDEE}" name="Table1" displayName="Table1" ref="A1:I29" totalsRowShown="0" headerRowDxfId="9">
+  <autoFilter ref="A1:I29" xr:uid="{B98D8822-403F-E442-BAE2-1B0B4CF679C4}"/>
+  <tableColumns count="9">
+    <tableColumn id="11" xr3:uid="{9CE7354F-C59C-2340-9022-92FB7EB9A5AB}" name="version" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{8CE13ACE-E9B8-3E47-8AF0-6D095CDC24CC}" name="target" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{51BF5B04-AEB1-434E-9660-5E7CFDD1FCEE}" name="flag" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{28841166-1611-7E4F-915D-75506BDADEB1}" name="p" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{19F13757-8028-F143-A57B-600899444B8A}" name="h0pz" dataDxfId="5"/>
     <tableColumn id="9" xr3:uid="{48BCA7F6-7248-AB4D-9D75-06481CBF62D3}" name="h1phiy" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{55FEDAD2-C7E8-AE41-A910-67C3EFFD93EB}" name="scale" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{6A1DDE75-7B5E-D54C-8F32-A21C08823890}" name="script" dataDxfId="2"/>
@@ -915,458 +951,857 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF8C9DC4-68D4-CB4E-900F-A4EA27E1DDD2}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="7" width="15.83203125" customWidth="1"/>
-    <col min="8" max="8" width="120.83203125" customWidth="1"/>
+    <col min="1" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="100.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E3" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E5" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="I5" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="1">
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="I7" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:9">
       <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E8" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="1">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:9">
       <c r="A9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="1">
         <v>1</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="I9" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:9">
       <c r="A10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E10" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="1">
         <v>1</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="H10" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="I10" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:9">
       <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
-      </c>
       <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="1">
         <v>1</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="I11" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:9">
       <c r="A12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="1">
+      <c r="F12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="1">
         <v>2</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:9">
       <c r="A13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="1">
+      <c r="F13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="1">
         <v>2</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:9">
       <c r="A14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="1">
+      <c r="F14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="1">
         <v>2</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="I14" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:9">
       <c r="A15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="1">
+      <c r="F15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="1">
         <v>2</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="H15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="I15" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:9">
       <c r="A16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="F16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="1">
         <v>2</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:9">
       <c r="A17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="1">
+      <c r="F17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="1">
         <v>2</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="H17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="I17" s="1" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="1">
+        <v>1</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" s="1">
+        <v>2</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G28" s="1">
+        <v>2</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="1">
+        <v>2</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>